<commit_message>
Data cleaning CBS done
</commit_message>
<xml_diff>
--- a/data/81071ned_metadata.xlsx
+++ b/data/81071ned_metadata.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eva/Documents/DataScience/data/Geneesmiddelen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eva/Documents/DataScience/Projecten/GeneesmiddelenCbs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EDDC45E-8682-A643-BEA8-B6A087DEB40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60467CC1-BE72-2947-9371-AE9BACF37E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="520" windowWidth="14400" windowHeight="17500"/>
+    <workbookView xWindow="1180" yWindow="520" windowWidth="14400" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leeftijd" sheetId="1" r:id="rId1"/>
     <sheet name="Geneesmiddelengroep" sheetId="2" r:id="rId2"/>
+    <sheet name="Geslacht" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="906">
   <si>
     <t>Title</t>
   </si>
@@ -2727,12 +2728,24 @@
   </si>
   <si>
     <t>Y Niet ingevuld</t>
+  </si>
+  <si>
+    <t>Vrouwen</t>
+  </si>
+  <si>
+    <t>Mannen</t>
+  </si>
+  <si>
+    <t>Totaal mannen en vrouwen</t>
+  </si>
+  <si>
+    <t>T001038</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3566,10 +3579,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -3817,7 +3830,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C378"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7212,4 +7225,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B334FC7-A146-F447-B05C-45356E8307AE}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>905</v>
+      </c>
+      <c r="B2" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4000</v>
+      </c>
+      <c r="B4" t="s">
+        <v>902</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>